<commit_message>
Update Deep Dive Deep Learning.xlsx
</commit_message>
<xml_diff>
--- a/Book-Deep Dive Deep Learning/Deep Dive Deep Learning.xlsx
+++ b/Book-Deep Dive Deep Learning/Deep Dive Deep Learning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\00_AI.Garden\01_Github\100_datSci\Book-Deep Dive Deep Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5022F2-4688-4ABE-9536-29E8E1D0F195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D107C0-4B1A-4AE1-BAA6-C0CA5B0F5B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{D56E7C0A-BCFF-45CB-898A-07DB1B86D966}"/>
   </bookViews>
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +134,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,12 +148,66 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -177,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -190,8 +251,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -511,7 +599,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,7 +622,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -542,7 +630,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -550,7 +638,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -558,7 +646,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+      <c r="A5" s="8">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -566,7 +654,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -574,7 +662,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="5">
+      <c r="A7" s="9">
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -582,7 +670,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -590,7 +678,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+      <c r="A9" s="9">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -598,23 +686,23 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="5">
-        <v>4</v>
+      <c r="A10" s="10">
+        <v>4.2</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>4</v>
+      <c r="A11" s="10">
+        <v>4.0999999999999996</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
+      <c r="A12" s="8">
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -622,7 +710,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
+      <c r="A13" s="15">
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -630,7 +718,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
+      <c r="A14" s="11">
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -638,7 +726,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+      <c r="A15" s="13">
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -646,7 +734,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
+      <c r="A16" s="13">
         <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -654,7 +742,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
+      <c r="A17" s="14">
         <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -662,7 +750,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="5">
+      <c r="A18" s="12">
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -670,7 +758,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="5">
+      <c r="A19" s="15">
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -678,7 +766,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
+      <c r="A20" s="12">
         <v>6</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -694,7 +782,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="5">
+      <c r="A22" s="7">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">

</xml_diff>